<commit_message>
grab # staff from excel sheet
</commit_message>
<xml_diff>
--- a/availability.xlsx
+++ b/availability.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\Life Scheduling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\GitHub\life-collegia-schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B9B80-42B9-4336-A7B4-CD5451A5DAFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765B2FD7-EBC2-484D-B2E3-1A6E115D561F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{750E1001-B131-4AD6-8EA9-0C913AF79012}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="22">
   <si>
     <t>Mon</t>
   </si>
@@ -72,7 +72,31 @@
     <t>Aa</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t># staff</t>
+  </si>
+  <si>
+    <t>Highly preferred</t>
+  </si>
+  <si>
+    <t>Slightly preferred</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Unpreferred</t>
+  </si>
+  <si>
+    <t>Travel time</t>
+  </si>
+  <si>
+    <t>Cannot work (unavailable)</t>
   </si>
 </sst>
 </file>
@@ -186,76 +210,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="64">
     <dxf>
       <font>
         <color theme="5" tint="-0.24994659260841701"/>
@@ -1125,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2444FAFD-DD66-4923-BB24-9F67C6E049D8}">
-  <dimension ref="A1:BC27"/>
+  <dimension ref="A1:BC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="AH19" sqref="AH19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4640,208 +4595,306 @@
         <v>-5</v>
       </c>
     </row>
+    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
     <row r="27" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="M27" t="s">
-        <v>13</v>
-      </c>
-      <c r="T27" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV27" t="s">
-        <v>13</v>
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1">
+        <v>-100</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A25:XFD1048576 U1:U24 AB1:AB24 AI1:XFD24 G1:N24">
-    <cfRule type="cellIs" dxfId="71" priority="107" operator="equal">
+  <conditionalFormatting sqref="U1:U24 AB1:AB24 AI1:XFD24 G1:N24 A25:XFD1048576">
+    <cfRule type="cellIs" dxfId="63" priority="107" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="108" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="109" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="110" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="111" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="208" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="209" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F24">
-    <cfRule type="cellIs" dxfId="64" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="61" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="62" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="63" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="64" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:T24">
-    <cfRule type="cellIs" dxfId="57" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:AA1 V8:AA16 V2:V6 V7:Z7 V17:Z24">
-    <cfRule type="cellIs" dxfId="50" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AH24">
-    <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="38" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="40" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:AA6">
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA17:AA24">
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4865,7 +4918,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A25:XFD1048576 U1:U24 AB1:AB24 AI1:XFD24 G1:N24</xm:sqref>
+          <xm:sqref>U1:U24 AB1:AB24 AI1:XFD24 G1:N24 A25:XFD1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="57" operator="containsText" id="{5AEB64F3-081F-4DF8-BB95-AE5E0CC64F79}">

</xml_diff>

<commit_message>
added xx placeholder staff member
</commit_message>
<xml_diff>
--- a/availability.xlsx
+++ b/availability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\GitHub\life-collegia-schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765B2FD7-EBC2-484D-B2E3-1A6E115D561F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6681C0C2-17F5-417F-AB4E-1852041CD933}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{750E1001-B131-4AD6-8EA9-0C913AF79012}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
   <si>
     <t>Mon</t>
   </si>
@@ -98,6 +98,15 @@
   <si>
     <t>Cannot work (unavailable)</t>
   </si>
+  <si>
+    <t>Xx</t>
+  </si>
+  <si>
+    <t>With Xx placeholder</t>
+  </si>
+  <si>
+    <t>Xx placeholder</t>
+  </si>
 </sst>
 </file>
 
@@ -121,7 +130,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +146,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -197,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -206,81 +221,18 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="240">
     <dxf>
       <font>
         <color theme="5" tint="-0.24994659260841701"/>
@@ -347,6 +299,1594 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1080,10 +2620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2444FAFD-DD66-4923-BB24-9F67C6E049D8}">
-  <dimension ref="A1:BC35"/>
+  <dimension ref="A1:BQ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,9 +2631,9 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1111,7 +2651,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>0</v>
@@ -1236,43 +2776,79 @@
       <c r="BC1" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="BE1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="BJ1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BM1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ1" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>5</v>
+      <c r="B2" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C2" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D2" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E2" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F2" s="10">
+        <v>-50</v>
       </c>
       <c r="H2" s="5">
         <v>0.33333333333333331</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J2" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="K2" s="1">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="L2" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="M2" s="2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O2" s="5">
         <v>0.33333333333333331</v>
@@ -1382,43 +2958,79 @@
       <c r="BC2" s="2">
         <v>-5</v>
       </c>
+      <c r="BE2" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="BF2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG2" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="2">
+        <v>5</v>
+      </c>
+      <c r="BL2" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN2" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>5</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ2" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>0.35416666666666669</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>4</v>
+      <c r="B3" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C3" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D3" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E3" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F3" s="10">
+        <v>-50</v>
       </c>
       <c r="H3" s="5">
         <v>0.35416666666666669</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J3" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="K3" s="1">
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="L3" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="M3" s="2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O3" s="5">
         <v>0.35416666666666669</v>
@@ -1528,43 +3140,79 @@
       <c r="BC3" s="2">
         <v>-5</v>
       </c>
+      <c r="BE3" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="BF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="2">
+        <v>4</v>
+      </c>
+      <c r="BL3" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="BM3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN3" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO3" s="1">
+        <v>4</v>
+      </c>
+      <c r="BP3" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>0.375</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3</v>
+      <c r="B4" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C4" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D4" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E4" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F4" s="10">
+        <v>-50</v>
       </c>
       <c r="H4" s="5">
         <v>0.375</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J4" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="K4" s="1">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="L4" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="M4" s="2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O4" s="5">
         <v>0.375</v>
@@ -1674,43 +3322,79 @@
       <c r="BC4" s="2">
         <v>-5</v>
       </c>
+      <c r="BE4" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="BF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG4" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="2">
+        <v>3</v>
+      </c>
+      <c r="BL4" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="BM4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN4" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO4" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP4" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ4" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2</v>
+      <c r="B5" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C5" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E5" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F5" s="10">
+        <v>-50</v>
       </c>
       <c r="H5" s="5">
         <v>0.39583333333333298</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J5" s="1">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="K5" s="1">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="L5" s="1">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="M5" s="2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O5" s="5">
         <v>0.39583333333333298</v>
@@ -1820,43 +3504,79 @@
       <c r="BC5" s="2">
         <v>-5</v>
       </c>
+      <c r="BE5" s="5">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="BF5" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG5" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH5" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="2">
+        <v>2</v>
+      </c>
+      <c r="BL5" s="5">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="BM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN5" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BO5" s="1">
+        <v>2</v>
+      </c>
+      <c r="BP5" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BQ5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
+      <c r="B6" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F6" s="10">
+        <v>-50</v>
       </c>
       <c r="H6" s="5">
         <v>0.41666666666666702</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="K6" s="1">
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="M6" s="2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O6" s="5">
         <v>0.41666666666666702</v>
@@ -1966,43 +3686,79 @@
       <c r="BC6" s="2">
         <v>-5</v>
       </c>
+      <c r="BE6" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="BF6" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG6" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH6" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ6" s="2">
+        <v>1</v>
+      </c>
+      <c r="BL6" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="BM6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BP6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ6" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>0.4375</v>
       </c>
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
+      <c r="B7" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D7" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E7" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F7" s="10">
+        <v>-50</v>
       </c>
       <c r="H7" s="5">
         <v>0.4375</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J7" s="1">
         <v>-99</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>-99</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O7" s="5">
         <v>0.4375</v>
@@ -2112,43 +3868,79 @@
       <c r="BC7" s="2">
         <v>-5</v>
       </c>
+      <c r="BE7" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="BF7" s="1">
+        <v>4</v>
+      </c>
+      <c r="BG7" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH7" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI7" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="BM7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BO7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ7" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B8" s="1">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
+      <c r="B8" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E8" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F8" s="10">
+        <v>-50</v>
       </c>
       <c r="H8" s="5">
         <v>0.45833333333333298</v>
       </c>
       <c r="I8" s="1">
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="J8" s="1">
         <v>-100</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L8" s="1">
         <v>-100</v>
       </c>
       <c r="M8" s="2">
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="O8" s="5">
         <v>0.45833333333333298</v>
@@ -2258,43 +4050,79 @@
       <c r="BC8" s="2">
         <v>-5</v>
       </c>
+      <c r="BE8" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="BF8" s="1">
+        <v>5</v>
+      </c>
+      <c r="BG8" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH8" s="1">
+        <v>5</v>
+      </c>
+      <c r="BI8" s="1">
+        <v>3</v>
+      </c>
+      <c r="BJ8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="BM8" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN8" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ8" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="1">
-        <v>-99</v>
-      </c>
-      <c r="C9" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-99</v>
-      </c>
-      <c r="E9" s="1">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2">
-        <v>-99</v>
+      <c r="B9" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C9" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D9" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E9" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F9" s="10">
+        <v>-50</v>
       </c>
       <c r="H9" s="5">
         <v>0.47916666666666702</v>
       </c>
       <c r="I9" s="1">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="J9" s="1">
         <v>-100</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L9" s="1">
         <v>-100</v>
       </c>
       <c r="M9" s="2">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="O9" s="5">
         <v>0.47916666666666702</v>
@@ -2404,43 +4232,79 @@
       <c r="BC9" s="2">
         <v>-5</v>
       </c>
+      <c r="BE9" s="5">
+        <v>0.47916666666666702</v>
+      </c>
+      <c r="BF9" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BG9" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH9" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BI9" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ9" s="2">
+        <v>-99</v>
+      </c>
+      <c r="BL9" s="5">
+        <v>0.47916666666666702</v>
+      </c>
+      <c r="BM9" s="1">
+        <v>2</v>
+      </c>
+      <c r="BN9" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP9" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ9" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>0.5</v>
       </c>
-      <c r="B10" s="1">
-        <v>-100</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D10" s="1">
-        <v>-100</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
-        <v>-100</v>
+      <c r="B10" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C10" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D10" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E10" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F10" s="10">
+        <v>-50</v>
       </c>
       <c r="H10" s="5">
         <v>0.5</v>
       </c>
       <c r="I10" s="1">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="J10" s="1">
         <v>-100</v>
       </c>
       <c r="K10" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L10" s="1">
         <v>-100</v>
       </c>
       <c r="M10" s="2">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="O10" s="5">
         <v>0.5</v>
@@ -2550,43 +4414,79 @@
       <c r="BC10" s="2">
         <v>-5</v>
       </c>
+      <c r="BE10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BF10" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BG10" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH10" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BI10" s="1">
+        <v>5</v>
+      </c>
+      <c r="BJ10" s="2">
+        <v>-100</v>
+      </c>
+      <c r="BL10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BM10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BN10" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO10" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP10" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ10" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B11" s="1">
-        <v>-100</v>
-      </c>
-      <c r="C11" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-100</v>
-      </c>
-      <c r="E11" s="1">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2">
-        <v>-100</v>
+      <c r="B11" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C11" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D11" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F11" s="10">
+        <v>-50</v>
       </c>
       <c r="H11" s="5">
         <v>0.52083333333333304</v>
       </c>
       <c r="I11" s="1">
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="J11" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="K11" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L11" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="M11" s="2">
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="O11" s="5">
         <v>0.52083333333333304</v>
@@ -2696,43 +4596,79 @@
       <c r="BC11" s="2">
         <v>-5</v>
       </c>
+      <c r="BE11" s="5">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="BF11" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BG11" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH11" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BI11" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ11" s="2">
+        <v>-100</v>
+      </c>
+      <c r="BL11" s="5">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="BM11" s="1">
+        <v>4</v>
+      </c>
+      <c r="BN11" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BO11" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP11" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BQ11" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="1">
-        <v>-100</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-100</v>
-      </c>
-      <c r="E12" s="1">
-        <v>3</v>
-      </c>
-      <c r="F12" s="2">
-        <v>-100</v>
+      <c r="B12" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C12" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D12" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E12" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F12" s="10">
+        <v>-50</v>
       </c>
       <c r="H12" s="5">
         <v>0.54166666666666696</v>
       </c>
       <c r="I12" s="1">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="J12" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="M12" s="2">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="O12" s="5">
         <v>0.54166666666666696</v>
@@ -2842,43 +4778,79 @@
       <c r="BC12" s="2">
         <v>-5</v>
       </c>
+      <c r="BE12" s="5">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="BF12" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BG12" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH12" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BI12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BJ12" s="2">
+        <v>-100</v>
+      </c>
+      <c r="BL12" s="5">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="BM12" s="1">
+        <v>5</v>
+      </c>
+      <c r="BN12" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO12" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP12" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ12" s="2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B13" s="1">
-        <v>-100</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-100</v>
-      </c>
-      <c r="E13" s="1">
-        <v>2</v>
-      </c>
-      <c r="F13" s="2">
-        <v>-100</v>
+      <c r="B13" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C13" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D13" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E13" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F13" s="10">
+        <v>-50</v>
       </c>
       <c r="H13" s="5">
         <v>0.5625</v>
       </c>
       <c r="I13" s="1">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="J13" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="K13" s="1">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="L13" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="M13" s="2">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="O13" s="5">
         <v>0.5625</v>
@@ -2988,43 +4960,79 @@
       <c r="BC13" s="2">
         <v>-5</v>
       </c>
+      <c r="BE13" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="BF13" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BG13" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH13" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BI13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ13" s="2">
+        <v>-100</v>
+      </c>
+      <c r="BL13" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="BM13" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BN13" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BO13" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BP13" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BQ13" s="2">
+        <v>-99</v>
+      </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B14" s="1">
-        <v>-100</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-100</v>
-      </c>
-      <c r="D14" s="1">
-        <v>-100</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <v>-100</v>
+      <c r="B14" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C14" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D14" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E14" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F14" s="10">
+        <v>-50</v>
       </c>
       <c r="H14" s="5">
         <v>0.58333333333333304</v>
       </c>
       <c r="I14" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="J14" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="K14" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="L14" s="1">
         <v>-100</v>
       </c>
       <c r="M14" s="2">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="O14" s="5">
         <v>0.58333333333333304</v>
@@ -3134,43 +5142,79 @@
       <c r="BC14" s="2">
         <v>-5</v>
       </c>
+      <c r="BE14" s="5">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="BF14" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BG14" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BH14" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BI14" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ14" s="2">
+        <v>-100</v>
+      </c>
+      <c r="BL14" s="5">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="BM14" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BN14" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO14" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BP14" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ14" s="2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B15" s="1">
-        <v>-100</v>
-      </c>
-      <c r="C15" s="1">
-        <v>-99</v>
-      </c>
-      <c r="D15" s="1">
-        <v>-100</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>-100</v>
+      <c r="B15" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C15" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D15" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E15" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F15" s="10">
+        <v>-50</v>
       </c>
       <c r="H15" s="5">
         <v>0.60416666666666696</v>
       </c>
       <c r="I15" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="J15" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="K15" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="L15" s="1">
         <v>-100</v>
       </c>
       <c r="M15" s="2">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="O15" s="5">
         <v>0.60416666666666696</v>
@@ -3280,43 +5324,79 @@
       <c r="BC15" s="2">
         <v>-5</v>
       </c>
+      <c r="BE15" s="5">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="BF15" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BG15" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BH15" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BI15" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ15" s="2">
+        <v>-100</v>
+      </c>
+      <c r="BL15" s="5">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="BM15" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BN15" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO15" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BP15" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ15" s="2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>0.625</v>
       </c>
-      <c r="B16" s="1">
-        <v>-100</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1">
-        <v>-100</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>-100</v>
+      <c r="B16" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C16" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D16" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E16" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F16" s="10">
+        <v>-50</v>
       </c>
       <c r="H16" s="5">
         <v>0.625</v>
       </c>
       <c r="I16" s="1">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="J16" s="1">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="K16" s="1">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="L16" s="1">
         <v>-100</v>
       </c>
       <c r="M16" s="2">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="O16" s="5">
         <v>0.625</v>
@@ -3426,43 +5506,79 @@
       <c r="BC16" s="2">
         <v>-5</v>
       </c>
+      <c r="BE16" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="BF16" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BG16" s="1">
+        <v>2</v>
+      </c>
+      <c r="BH16" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BI16" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="2">
+        <v>-100</v>
+      </c>
+      <c r="BL16" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="BM16" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BN16" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BO16" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BP16" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BQ16" s="2">
+        <v>-99</v>
+      </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>0.64583333333333404</v>
       </c>
-      <c r="B17" s="1">
-        <v>-100</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1">
-        <v>-100</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>-100</v>
+      <c r="B17" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C17" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D17" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E17" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F17" s="10">
+        <v>-50</v>
       </c>
       <c r="H17" s="5">
         <v>0.64583333333333404</v>
       </c>
       <c r="I17" s="1">
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="J17" s="1">
-        <v>-99</v>
+        <v>-5</v>
       </c>
       <c r="K17" s="1">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="L17" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="M17" s="2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O17" s="5">
         <v>0.64583333333333404</v>
@@ -3572,43 +5688,79 @@
       <c r="BC17" s="2">
         <v>-5</v>
       </c>
+      <c r="BE17" s="5">
+        <v>0.64583333333333404</v>
+      </c>
+      <c r="BF17" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BG17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH17" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BI17" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ17" s="2">
+        <v>-100</v>
+      </c>
+      <c r="BL17" s="5">
+        <v>0.64583333333333404</v>
+      </c>
+      <c r="BM17" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN17" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BO17" s="1">
+        <v>5</v>
+      </c>
+      <c r="BP17" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BQ17" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="1">
-        <v>-99</v>
-      </c>
-      <c r="C18" s="1">
-        <v>4</v>
-      </c>
-      <c r="D18" s="1">
-        <v>-99</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>-99</v>
+      <c r="B18" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C18" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D18" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E18" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F18" s="10">
+        <v>-50</v>
       </c>
       <c r="H18" s="5">
         <v>0.66666666666666696</v>
       </c>
       <c r="I18" s="1">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="J18" s="1">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="K18" s="1">
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="L18" s="1">
-        <v>5</v>
+        <v>-100</v>
       </c>
       <c r="M18" s="2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O18" s="5">
         <v>0.66666666666666696</v>
@@ -3718,43 +5870,79 @@
       <c r="BC18" s="2">
         <v>-5</v>
       </c>
+      <c r="BE18" s="5">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="BF18" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BG18" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH18" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BI18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ18" s="2">
+        <v>-99</v>
+      </c>
+      <c r="BL18" s="5">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="BM18" s="1">
+        <v>2</v>
+      </c>
+      <c r="BN18" s="1">
+        <v>5</v>
+      </c>
+      <c r="BO18" s="1">
+        <v>4</v>
+      </c>
+      <c r="BP18" s="1">
+        <v>5</v>
+      </c>
+      <c r="BQ18" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>0.6875</v>
       </c>
-      <c r="B19" s="1">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1">
-        <v>-99</v>
-      </c>
-      <c r="F19" s="2">
-        <v>-5</v>
+      <c r="B19" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C19" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D19" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E19" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F19" s="10">
+        <v>-50</v>
       </c>
       <c r="H19" s="5">
         <v>0.6875</v>
       </c>
       <c r="I19" s="1">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="J19" s="1">
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="K19" s="1">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="L19" s="1">
-        <v>4</v>
+        <v>-100</v>
       </c>
       <c r="M19" s="2">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="O19" s="5">
         <v>0.6875</v>
@@ -3864,43 +6052,79 @@
       <c r="BC19" s="2">
         <v>-5</v>
       </c>
+      <c r="BE19" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="BF19" s="1">
+        <v>5</v>
+      </c>
+      <c r="BG19" s="1">
+        <v>5</v>
+      </c>
+      <c r="BH19" s="1">
+        <v>5</v>
+      </c>
+      <c r="BI19" s="1">
+        <v>-99</v>
+      </c>
+      <c r="BJ19" s="2">
+        <v>-5</v>
+      </c>
+      <c r="BL19" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="BM19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BN19" s="1">
+        <v>4</v>
+      </c>
+      <c r="BO19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP19" s="1">
+        <v>4</v>
+      </c>
+      <c r="BQ19" s="2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B20" s="1">
-        <v>4</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1">
-        <v>4</v>
-      </c>
-      <c r="E20" s="1">
-        <v>-100</v>
-      </c>
-      <c r="F20" s="2">
-        <v>-5</v>
+      <c r="B20" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C20" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D20" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E20" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F20" s="10">
+        <v>-50</v>
       </c>
       <c r="H20" s="5">
         <v>0.70833333333333404</v>
       </c>
       <c r="I20" s="1">
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="J20" s="1">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="K20" s="1">
-        <v>2</v>
+        <v>-99</v>
       </c>
       <c r="L20" s="1">
-        <v>3</v>
+        <v>-99</v>
       </c>
       <c r="M20" s="2">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="O20" s="5">
         <v>0.70833333333333404</v>
@@ -4010,43 +6234,79 @@
       <c r="BC20" s="2">
         <v>-5</v>
       </c>
+      <c r="BE20" s="5">
+        <v>0.70833333333333404</v>
+      </c>
+      <c r="BF20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BG20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI20" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BJ20" s="2">
+        <v>-5</v>
+      </c>
+      <c r="BL20" s="5">
+        <v>0.70833333333333404</v>
+      </c>
+      <c r="BM20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BN20" s="1">
+        <v>3</v>
+      </c>
+      <c r="BO20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BP20" s="1">
+        <v>3</v>
+      </c>
+      <c r="BQ20" s="2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>0.72916666666666696</v>
       </c>
-      <c r="B21" s="1">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1">
-        <v>-100</v>
-      </c>
-      <c r="F21" s="2">
-        <v>-5</v>
+      <c r="B21" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C21" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D21" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E21" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F21" s="10">
+        <v>-50</v>
       </c>
       <c r="H21" s="5">
         <v>0.72916666666666696</v>
       </c>
       <c r="I21" s="1">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="J21" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="K21" s="1">
         <v>-100</v>
       </c>
       <c r="L21" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="M21" s="2">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="O21" s="5">
         <v>0.72916666666666696</v>
@@ -4156,43 +6416,79 @@
       <c r="BC21" s="2">
         <v>-5</v>
       </c>
+      <c r="BE21" s="5">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="BF21" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG21" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH21" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI21" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BJ21" s="2">
+        <v>-5</v>
+      </c>
+      <c r="BL21" s="5">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="BM21" s="1">
+        <v>5</v>
+      </c>
+      <c r="BN21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO21" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BP21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ21" s="2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>0.75</v>
       </c>
-      <c r="B22" s="1">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>-100</v>
-      </c>
-      <c r="F22" s="2">
-        <v>-5</v>
+      <c r="B22" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C22" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D22" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E22" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F22" s="10">
+        <v>-50</v>
       </c>
       <c r="H22" s="5">
         <v>0.75</v>
       </c>
       <c r="I22" s="1">
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="K22" s="1">
         <v>-100</v>
       </c>
       <c r="L22" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="M22" s="2">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="O22" s="5">
         <v>0.75</v>
@@ -4302,43 +6598,79 @@
       <c r="BC22" s="2">
         <v>-5</v>
       </c>
+      <c r="BE22" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="BF22" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG22" s="1">
+        <v>2</v>
+      </c>
+      <c r="BH22" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI22" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BJ22" s="2">
+        <v>-5</v>
+      </c>
+      <c r="BL22" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="BM22" s="1">
+        <v>4</v>
+      </c>
+      <c r="BN22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO22" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BP22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ22" s="2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>0.77083333333333404</v>
       </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <v>-100</v>
-      </c>
-      <c r="F23" s="2">
-        <v>-5</v>
+      <c r="B23" s="9">
+        <v>-50</v>
+      </c>
+      <c r="C23" s="9">
+        <v>-50</v>
+      </c>
+      <c r="D23" s="9">
+        <v>-50</v>
+      </c>
+      <c r="E23" s="9">
+        <v>-50</v>
+      </c>
+      <c r="F23" s="10">
+        <v>-50</v>
       </c>
       <c r="H23" s="5">
         <v>0.77083333333333404</v>
       </c>
       <c r="I23" s="1">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="K23" s="1">
         <v>-100</v>
       </c>
       <c r="L23" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="M23" s="2">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="O23" s="5">
         <v>0.77083333333333404</v>
@@ -4448,43 +6780,79 @@
       <c r="BC23" s="2">
         <v>-5</v>
       </c>
+      <c r="BE23" s="5">
+        <v>0.77083333333333404</v>
+      </c>
+      <c r="BF23" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG23" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH23" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI23" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BJ23" s="2">
+        <v>-5</v>
+      </c>
+      <c r="BL23" s="5">
+        <v>0.77083333333333404</v>
+      </c>
+      <c r="BM23" s="1">
+        <v>3</v>
+      </c>
+      <c r="BN23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO23" s="1">
+        <v>-100</v>
+      </c>
+      <c r="BP23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ23" s="2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="24" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B24" s="3">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
-        <v>-100</v>
-      </c>
-      <c r="F24" s="4">
-        <v>-5</v>
+      <c r="B24" s="11">
+        <v>-50</v>
+      </c>
+      <c r="C24" s="11">
+        <v>-50</v>
+      </c>
+      <c r="D24" s="11">
+        <v>-50</v>
+      </c>
+      <c r="E24" s="11">
+        <v>-50</v>
+      </c>
+      <c r="F24" s="12">
+        <v>-50</v>
       </c>
       <c r="H24" s="5">
         <v>0.79166666666666696</v>
       </c>
       <c r="I24" s="3">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="J24" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="K24" s="3">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="L24" s="3">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="M24" s="4">
-        <v>-100</v>
+        <v>-5</v>
       </c>
       <c r="O24" s="5">
         <v>0.79166666666666696</v>
@@ -4594,308 +6962,417 @@
       <c r="BC24" s="4">
         <v>-5</v>
       </c>
+      <c r="BE24" s="5">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="BF24" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG24" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH24" s="3">
+        <v>0</v>
+      </c>
+      <c r="BI24" s="3">
+        <v>-100</v>
+      </c>
+      <c r="BJ24" s="4">
+        <v>-5</v>
+      </c>
+      <c r="BL24" s="5">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="BM24" s="3">
+        <v>2</v>
+      </c>
+      <c r="BN24" s="3">
+        <v>0</v>
+      </c>
+      <c r="BO24" s="3">
+        <v>-100</v>
+      </c>
+      <c r="BP24" s="3">
+        <v>0</v>
+      </c>
+      <c r="BQ24" s="4">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="8"/>
+      <c r="C27" s="1">
         <v>8</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+    <row r="28" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="1">
+        <f>C27 + 1</f>
+        <v>9</v>
+      </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1">
         <v>-5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1">
         <v>-99</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1">
-        <v>-100</v>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="1">
+        <v>-50</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="U1:U24 AB1:AB24 AI1:XFD24 G1:N24 A25:XFD1048576">
-    <cfRule type="cellIs" dxfId="63" priority="107" operator="equal">
+  <mergeCells count="2">
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+  </mergeCells>
+  <conditionalFormatting sqref="U1:U24 AB1:AB24 AI1:BD24 BR1:XFD24 G1:N24 A27:A28 A25:XFD25 A26:C26 E26:XFD35 A36:XFD1048576 A29:C35 C27:C28">
+    <cfRule type="cellIs" dxfId="159" priority="139" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="140" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="141" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="142" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="143" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="240" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="241" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:AA1 V8:AA16 V2:V6 V7:Z7 V17:Z24">
+    <cfRule type="cellIs" dxfId="152" priority="74" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="75" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="76" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="77" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="78" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="79" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="80" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:T24">
+    <cfRule type="cellIs" dxfId="145" priority="82" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="83" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="84" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="85" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="86" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="87" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="88" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC1:AH24">
+    <cfRule type="cellIs" dxfId="138" priority="66" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="67" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="68" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="69" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="70" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="71" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="72" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:AA6">
+    <cfRule type="cellIs" dxfId="131" priority="58" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="59" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="60" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="61" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="62" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="63" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="64" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA17:AA24">
+    <cfRule type="cellIs" dxfId="124" priority="42" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="43" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="44" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="45" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="46" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="47" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="48" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA7">
+    <cfRule type="cellIs" dxfId="117" priority="34" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="35" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="36" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="37" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="38" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="39" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="111" priority="40" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U24 AB1:AB24 AI1:BD24 BR1:XFD24 G1:N24 A27:A28 A25:XFD25 A26:C26 E26:XFD35 A36:XFD1048576 A29:C35 C27:C28">
+    <cfRule type="cellIs" dxfId="110" priority="105" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BK1:BQ24">
+    <cfRule type="cellIs" dxfId="103" priority="26" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="27" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="28" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="29" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="30" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="31" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="32" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BE1:BJ24">
+    <cfRule type="cellIs" dxfId="96" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="19" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="20" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="21" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="22" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="23" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="24" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F24">
-    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="6" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="7" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="8" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T24">
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
-      <formula>-99</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
-      <formula>-100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V1:AA1 V8:AA16 V2:V6 V7:Z7 V17:Z24">
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
-      <formula>-99</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
-      <formula>-100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC1:AH24">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="38" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
-      <formula>-99</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="40" operator="equal">
-      <formula>-100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W2:AA6">
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
-      <formula>-99</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
-      <formula>-100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA17:AA24">
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
-      <formula>-99</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
-      <formula>-100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA7">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
-      <formula>-99</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>-100</formula>
+  <conditionalFormatting sqref="A1:F24">
+    <cfRule type="cellIs" dxfId="80" priority="1" operator="equal">
+      <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4904,8 +7381,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="73" operator="containsText" id="{FE65B820-67A6-4FF8-87D1-482B072706B5}">
-            <xm:f>NOT(ISERROR(SEARCH(-5,A1)))</xm:f>
+          <x14:cfRule type="containsText" priority="73" operator="containsText" id="{5AEB64F3-081F-4DF8-BB95-AE5E0CC64F79}">
+            <xm:f>NOT(ISERROR(SEARCH(-5,V1)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
               <font>
@@ -4918,27 +7395,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>U1:U24 AB1:AB24 AI1:XFD24 G1:N24 A25:XFD1048576</xm:sqref>
+          <xm:sqref>V1:AA1 V8:AA16 V2:V6 V7:Z7 V17:Z24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="57" operator="containsText" id="{5AEB64F3-081F-4DF8-BB95-AE5E0CC64F79}">
-            <xm:f>NOT(ISERROR(SEARCH(-5,A1)))</xm:f>
-            <xm:f>-5</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="5" tint="-0.24994659260841701"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:F24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="49" operator="containsText" id="{9C988215-61F1-4CAD-8003-ED597D45813D}">
+          <x14:cfRule type="containsText" priority="81" operator="containsText" id="{9C988215-61F1-4CAD-8003-ED597D45813D}">
             <xm:f>NOT(ISERROR(SEARCH(-5,O1)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
@@ -4955,24 +7415,7 @@
           <xm:sqref>O1:T24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="41" operator="containsText" id="{98B34D08-8BF6-4894-A9CA-3E0D57CA1103}">
-            <xm:f>NOT(ISERROR(SEARCH(-5,V1)))</xm:f>
-            <xm:f>-5</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="5" tint="-0.24994659260841701"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.79998168889431442"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>V1:AA1 V8:AA16 V2:V6 V7:Z7 V17:Z24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="33" operator="containsText" id="{E147DA2D-ACE5-47A4-8421-F6F7A823AD8F}">
+          <x14:cfRule type="containsText" priority="65" operator="containsText" id="{E147DA2D-ACE5-47A4-8421-F6F7A823AD8F}">
             <xm:f>NOT(ISERROR(SEARCH(-5,AC1)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
@@ -4989,7 +7432,7 @@
           <xm:sqref>AC1:AH24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{D33E7692-5BD1-4288-8D52-AA683F6CA264}">
+          <x14:cfRule type="containsText" priority="57" operator="containsText" id="{D33E7692-5BD1-4288-8D52-AA683F6CA264}">
             <xm:f>NOT(ISERROR(SEARCH(-5,W2)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
@@ -5006,7 +7449,7 @@
           <xm:sqref>W2:AA6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{08F50A8E-4C65-4990-9515-037D07F60F25}">
+          <x14:cfRule type="containsText" priority="41" operator="containsText" id="{08F50A8E-4C65-4990-9515-037D07F60F25}">
             <xm:f>NOT(ISERROR(SEARCH(-5,AA17)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
@@ -5023,7 +7466,7 @@
           <xm:sqref>AA17:AA24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{993DE8D1-17A9-4790-81D7-170B68296247}">
+          <x14:cfRule type="containsText" priority="33" operator="containsText" id="{993DE8D1-17A9-4790-81D7-170B68296247}">
             <xm:f>NOT(ISERROR(SEARCH(-5,AA7)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
@@ -5039,6 +7482,40 @@
           </x14:cfRule>
           <xm:sqref>AA7</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{DC4F45F0-A295-4ED3-97E0-2C38404DEA26}">
+            <xm:f>NOT(ISERROR(SEARCH(-5,BK1)))</xm:f>
+            <xm:f>-5</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="5" tint="-0.24994659260841701"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>BK1:BQ24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{64681BE5-62F0-4BE2-B713-DF3D34ECA7EB}">
+            <xm:f>NOT(ISERROR(SEARCH(-5,BE1)))</xm:f>
+            <xm:f>-5</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="5" tint="-0.24994659260841701"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>BE1:BJ24</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
initial test and update of ranges for placeholder
</commit_message>
<xml_diff>
--- a/availability.xlsx
+++ b/availability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\GitHub\life-collegia-schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6681C0C2-17F5-417F-AB4E-1852041CD933}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32823DE2-3594-499A-9A09-73F67BC511BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{750E1001-B131-4AD6-8EA9-0C913AF79012}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>Mon</t>
   </si>
@@ -221,18 +221,98 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="240">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="5" tint="-0.24994659260841701"/>
@@ -304,26 +384,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -437,1446 +497,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5E913B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4F7EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2620,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2444FAFD-DD66-4923-BB24-9F67C6E049D8}">
-  <dimension ref="A1:BQ36"/>
+  <dimension ref="A1:BJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2631,7 +1251,7 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -2759,7 +1379,7 @@
         <v>4</v>
       </c>
       <c r="AX1" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AY1" s="6" t="s">
         <v>0</v>
@@ -2777,7 +1397,7 @@
         <v>4</v>
       </c>
       <c r="BE1" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF1" s="6" t="s">
         <v>0</v>
@@ -2794,42 +1414,24 @@
       <c r="BJ1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="BL1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BM1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="BN1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="BO1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BP1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="BQ1" s="6" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C2" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D2" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E2" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F2" s="10">
+      <c r="B2" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C2" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D2" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E2" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F2" s="9">
         <v>-50</v>
       </c>
       <c r="H2" s="5">
@@ -2944,19 +1546,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AY2" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="AZ2" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BA2" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BB2" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="BE2" s="5">
         <v>0.33333333333333331</v>
@@ -2968,50 +1570,32 @@
         <v>-100</v>
       </c>
       <c r="BH2" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BI2" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="BJ2" s="2">
-        <v>5</v>
-      </c>
-      <c r="BL2" s="5">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="BM2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN2" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO2" s="1">
-        <v>5</v>
-      </c>
-      <c r="BP2" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>0.35416666666666669</v>
       </c>
-      <c r="B3" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C3" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D3" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E3" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="B3" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C3" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D3" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E3" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F3" s="9">
         <v>-50</v>
       </c>
       <c r="H3" s="5">
@@ -3126,19 +1710,19 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="AY3" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="AZ3" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BA3" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BB3" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="BE3" s="5">
         <v>0.35416666666666669</v>
@@ -3150,50 +1734,32 @@
         <v>-100</v>
       </c>
       <c r="BH3" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BI3" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="BJ3" s="2">
-        <v>4</v>
-      </c>
-      <c r="BL3" s="5">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="BM3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN3" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO3" s="1">
-        <v>4</v>
-      </c>
-      <c r="BP3" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>0.375</v>
       </c>
-      <c r="B4" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C4" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D4" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E4" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F4" s="10">
+      <c r="B4" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C4" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D4" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E4" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F4" s="9">
         <v>-50</v>
       </c>
       <c r="H4" s="5">
@@ -3308,74 +1874,56 @@
         <v>0.375</v>
       </c>
       <c r="AY4" s="1">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="AZ4" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BA4" s="1">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="BB4" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BC4" s="2">
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="BE4" s="5">
         <v>0.375</v>
       </c>
       <c r="BF4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG4" s="1">
         <v>-100</v>
       </c>
       <c r="BH4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BI4" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="BJ4" s="2">
-        <v>3</v>
-      </c>
-      <c r="BL4" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="BM4" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN4" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO4" s="1">
-        <v>3</v>
-      </c>
-      <c r="BP4" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B5" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C5" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D5" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E5" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F5" s="10">
+      <c r="B5" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C5" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D5" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E5" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F5" s="9">
         <v>-50</v>
       </c>
       <c r="H5" s="5">
@@ -3490,74 +2038,56 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="AY5" s="1">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="AZ5" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BA5" s="1">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="BB5" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BC5" s="2">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="BE5" s="5">
         <v>0.39583333333333298</v>
       </c>
       <c r="BF5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BG5" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BH5" s="1">
         <v>2</v>
       </c>
       <c r="BI5" s="1">
-        <v>0</v>
+        <v>-99</v>
       </c>
       <c r="BJ5" s="2">
-        <v>2</v>
-      </c>
-      <c r="BL5" s="5">
-        <v>0.39583333333333298</v>
-      </c>
-      <c r="BM5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN5" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BO5" s="1">
-        <v>2</v>
-      </c>
-      <c r="BP5" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BQ5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B6" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C6" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D6" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E6" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="B6" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C6" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D6" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E6" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F6" s="9">
         <v>-50</v>
       </c>
       <c r="H6" s="5">
@@ -3672,74 +2202,56 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="AY6" s="1">
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="AZ6" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BA6" s="1">
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="BB6" s="1">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="BC6" s="2">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="BE6" s="5">
         <v>0.41666666666666702</v>
       </c>
       <c r="BF6" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BG6" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BH6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BI6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ6" s="2">
-        <v>1</v>
-      </c>
-      <c r="BL6" s="5">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="BM6" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN6" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO6" s="1">
-        <v>1</v>
-      </c>
-      <c r="BP6" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>0.4375</v>
       </c>
-      <c r="B7" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C7" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D7" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E7" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F7" s="10">
+      <c r="B7" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C7" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D7" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E7" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F7" s="9">
         <v>-50</v>
       </c>
       <c r="H7" s="5">
@@ -3854,74 +2366,56 @@
         <v>0.4375</v>
       </c>
       <c r="AY7" s="1">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="AZ7" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="BA7" s="1">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="BB7" s="1">
-        <v>-99</v>
+        <v>2</v>
       </c>
       <c r="BC7" s="2">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BE7" s="5">
         <v>0.4375</v>
       </c>
       <c r="BF7" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BG7" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BH7" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BI7" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BJ7" s="2">
         <v>0</v>
       </c>
-      <c r="BL7" s="5">
-        <v>0.4375</v>
-      </c>
-      <c r="BM7" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN7" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BO7" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP7" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ7" s="2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B8" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C8" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D8" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E8" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="B8" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C8" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D8" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E8" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F8" s="9">
         <v>-50</v>
       </c>
       <c r="H8" s="5">
@@ -4036,74 +2530,56 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="AY8" s="1">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="AZ8" s="1">
         <v>-100</v>
       </c>
       <c r="BA8" s="1">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="BB8" s="1">
-        <v>-100</v>
+        <v>3</v>
       </c>
       <c r="BC8" s="2">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BE8" s="5">
         <v>0.45833333333333298</v>
       </c>
       <c r="BF8" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BG8" s="1">
         <v>-100</v>
       </c>
       <c r="BH8" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BI8" s="1">
-        <v>3</v>
+        <v>-100</v>
       </c>
       <c r="BJ8" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="5">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="BM8" s="1">
         <v>1</v>
       </c>
-      <c r="BN8" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO8" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP8" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ8" s="2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C9" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D9" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E9" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="B9" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C9" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D9" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E9" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F9" s="9">
         <v>-50</v>
       </c>
       <c r="H9" s="5">
@@ -4218,74 +2694,56 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="AY9" s="1">
-        <v>-5</v>
+        <v>-99</v>
       </c>
       <c r="AZ9" s="1">
         <v>-100</v>
       </c>
       <c r="BA9" s="1">
-        <v>-5</v>
+        <v>-99</v>
       </c>
       <c r="BB9" s="1">
-        <v>-100</v>
+        <v>4</v>
       </c>
       <c r="BC9" s="2">
-        <v>-5</v>
+        <v>-99</v>
       </c>
       <c r="BE9" s="5">
         <v>0.47916666666666702</v>
       </c>
       <c r="BF9" s="1">
-        <v>-99</v>
+        <v>2</v>
       </c>
       <c r="BG9" s="1">
         <v>-100</v>
       </c>
       <c r="BH9" s="1">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="BI9" s="1">
-        <v>4</v>
+        <v>-100</v>
       </c>
       <c r="BJ9" s="2">
-        <v>-99</v>
-      </c>
-      <c r="BL9" s="5">
-        <v>0.47916666666666702</v>
-      </c>
-      <c r="BM9" s="1">
         <v>2</v>
       </c>
-      <c r="BN9" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO9" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP9" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ9" s="2">
-        <v>2</v>
-      </c>
     </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>0.5</v>
       </c>
-      <c r="B10" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C10" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D10" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E10" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="B10" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C10" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D10" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E10" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F10" s="9">
         <v>-50</v>
       </c>
       <c r="H10" s="5">
@@ -4400,74 +2858,56 @@
         <v>0.5</v>
       </c>
       <c r="AY10" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="AZ10" s="1">
         <v>-100</v>
       </c>
       <c r="BA10" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BB10" s="1">
-        <v>-100</v>
+        <v>5</v>
       </c>
       <c r="BC10" s="2">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BE10" s="5">
         <v>0.5</v>
       </c>
       <c r="BF10" s="1">
-        <v>-100</v>
+        <v>3</v>
       </c>
       <c r="BG10" s="1">
         <v>-100</v>
       </c>
       <c r="BH10" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BI10" s="1">
-        <v>5</v>
+        <v>-100</v>
       </c>
       <c r="BJ10" s="2">
-        <v>-100</v>
-      </c>
-      <c r="BL10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="BM10" s="1">
         <v>3</v>
       </c>
-      <c r="BN10" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO10" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP10" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ10" s="2">
-        <v>3</v>
-      </c>
     </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B11" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C11" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D11" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E11" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F11" s="10">
+      <c r="B11" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C11" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D11" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E11" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F11" s="9">
         <v>-50</v>
       </c>
       <c r="H11" s="5">
@@ -4582,74 +3022,56 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="AY11" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="AZ11" s="1">
         <v>-100</v>
       </c>
       <c r="BA11" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BB11" s="1">
-        <v>-100</v>
+        <v>4</v>
       </c>
       <c r="BC11" s="2">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BE11" s="5">
         <v>0.52083333333333304</v>
       </c>
       <c r="BF11" s="1">
-        <v>-100</v>
+        <v>4</v>
       </c>
       <c r="BG11" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BH11" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BI11" s="1">
-        <v>4</v>
+        <v>-99</v>
       </c>
       <c r="BJ11" s="2">
-        <v>-100</v>
-      </c>
-      <c r="BL11" s="5">
-        <v>0.52083333333333304</v>
-      </c>
-      <c r="BM11" s="1">
-        <v>4</v>
-      </c>
-      <c r="BN11" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BO11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP11" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BQ11" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C12" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D12" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E12" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F12" s="10">
+      <c r="B12" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C12" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D12" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E12" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F12" s="9">
         <v>-50</v>
       </c>
       <c r="H12" s="5">
@@ -4764,74 +3186,56 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="AY12" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="AZ12" s="1">
         <v>-100</v>
       </c>
       <c r="BA12" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BB12" s="1">
-        <v>-100</v>
+        <v>3</v>
       </c>
       <c r="BC12" s="2">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BE12" s="5">
         <v>0.54166666666666696</v>
       </c>
       <c r="BF12" s="1">
-        <v>-100</v>
+        <v>5</v>
       </c>
       <c r="BG12" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BH12" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BI12" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BJ12" s="2">
-        <v>-100</v>
-      </c>
-      <c r="BL12" s="5">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="BM12" s="1">
         <v>5</v>
       </c>
-      <c r="BN12" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO12" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP12" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ12" s="2">
-        <v>5</v>
-      </c>
     </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B13" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C13" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D13" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E13" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F13" s="10">
+      <c r="B13" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D13" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E13" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F13" s="9">
         <v>-50</v>
       </c>
       <c r="H13" s="5">
@@ -4946,74 +3350,56 @@
         <v>0.5625</v>
       </c>
       <c r="AY13" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="AZ13" s="1">
         <v>-100</v>
       </c>
       <c r="BA13" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BB13" s="1">
-        <v>-100</v>
+        <v>2</v>
       </c>
       <c r="BC13" s="2">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BE13" s="5">
         <v>0.5625</v>
       </c>
       <c r="BF13" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BG13" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BH13" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BI13" s="1">
-        <v>2</v>
+        <v>-99</v>
       </c>
       <c r="BJ13" s="2">
-        <v>-100</v>
-      </c>
-      <c r="BL13" s="5">
-        <v>0.5625</v>
-      </c>
-      <c r="BM13" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BN13" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BO13" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BP13" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BQ13" s="2">
         <v>-99</v>
       </c>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B14" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C14" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D14" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E14" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F14" s="10">
+      <c r="B14" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C14" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D14" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E14" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F14" s="9">
         <v>-50</v>
       </c>
       <c r="H14" s="5">
@@ -5128,19 +3514,19 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="AY14" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="AZ14" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="BA14" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BB14" s="1">
-        <v>-100</v>
+        <v>1</v>
       </c>
       <c r="BC14" s="2">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BE14" s="5">
         <v>0.58333333333333304</v>
@@ -5155,47 +3541,29 @@
         <v>-100</v>
       </c>
       <c r="BI14" s="1">
-        <v>1</v>
+        <v>-100</v>
       </c>
       <c r="BJ14" s="2">
         <v>-100</v>
       </c>
-      <c r="BL14" s="5">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="BM14" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BN14" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO14" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BP14" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ14" s="2">
-        <v>-100</v>
-      </c>
     </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B15" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C15" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D15" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E15" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F15" s="10">
+      <c r="B15" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C15" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D15" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E15" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F15" s="9">
         <v>-50</v>
       </c>
       <c r="H15" s="5">
@@ -5310,19 +3678,19 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="AY15" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="AZ15" s="1">
-        <v>-5</v>
+        <v>-99</v>
       </c>
       <c r="BA15" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BB15" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BC15" s="2">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BE15" s="5">
         <v>0.60416666666666696</v>
@@ -5331,53 +3699,35 @@
         <v>-100</v>
       </c>
       <c r="BG15" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="BH15" s="1">
         <v>-100</v>
       </c>
       <c r="BI15" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="BJ15" s="2">
         <v>-100</v>
       </c>
-      <c r="BL15" s="5">
-        <v>0.60416666666666696</v>
-      </c>
-      <c r="BM15" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BN15" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO15" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BP15" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ15" s="2">
-        <v>-100</v>
-      </c>
     </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>0.625</v>
       </c>
-      <c r="B16" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C16" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D16" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E16" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F16" s="10">
+      <c r="B16" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C16" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D16" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E16" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F16" s="9">
         <v>-50</v>
       </c>
       <c r="H16" s="5">
@@ -5492,74 +3842,56 @@
         <v>0.625</v>
       </c>
       <c r="AY16" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="AZ16" s="1">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="BA16" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BB16" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BC16" s="2">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BE16" s="5">
         <v>0.625</v>
       </c>
       <c r="BF16" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BG16" s="1">
-        <v>2</v>
+        <v>-100</v>
       </c>
       <c r="BH16" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BI16" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="BJ16" s="2">
-        <v>-100</v>
-      </c>
-      <c r="BL16" s="5">
-        <v>0.625</v>
-      </c>
-      <c r="BM16" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BN16" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BO16" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BP16" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BQ16" s="2">
         <v>-99</v>
       </c>
     </row>
-    <row r="17" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>0.64583333333333404</v>
       </c>
-      <c r="B17" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C17" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D17" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E17" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F17" s="10">
+      <c r="B17" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C17" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D17" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F17" s="9">
         <v>-50</v>
       </c>
       <c r="H17" s="5">
@@ -5674,74 +4006,56 @@
         <v>0.64583333333333404</v>
       </c>
       <c r="AY17" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="AZ17" s="1">
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="BA17" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BB17" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BC17" s="2">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BE17" s="5">
         <v>0.64583333333333404</v>
       </c>
       <c r="BF17" s="1">
-        <v>-100</v>
+        <v>1</v>
       </c>
       <c r="BG17" s="1">
-        <v>3</v>
+        <v>-99</v>
       </c>
       <c r="BH17" s="1">
-        <v>-100</v>
+        <v>5</v>
       </c>
       <c r="BI17" s="1">
-        <v>0</v>
+        <v>-99</v>
       </c>
       <c r="BJ17" s="2">
-        <v>-100</v>
-      </c>
-      <c r="BL17" s="5">
-        <v>0.64583333333333404</v>
-      </c>
-      <c r="BM17" s="1">
-        <v>1</v>
-      </c>
-      <c r="BN17" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BO17" s="1">
-        <v>5</v>
-      </c>
-      <c r="BP17" s="1">
-        <v>-99</v>
-      </c>
-      <c r="BQ17" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C18" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D18" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E18" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F18" s="10">
+      <c r="B18" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C18" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D18" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E18" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F18" s="9">
         <v>-50</v>
       </c>
       <c r="H18" s="5">
@@ -5856,74 +4170,56 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="AY18" s="1">
-        <v>-5</v>
+        <v>-99</v>
       </c>
       <c r="AZ18" s="1">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="BA18" s="1">
-        <v>-5</v>
+        <v>-99</v>
       </c>
       <c r="BB18" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BC18" s="2">
-        <v>-5</v>
+        <v>-99</v>
       </c>
       <c r="BE18" s="5">
         <v>0.66666666666666696</v>
       </c>
       <c r="BF18" s="1">
-        <v>-99</v>
+        <v>2</v>
       </c>
       <c r="BG18" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BH18" s="1">
-        <v>-99</v>
+        <v>4</v>
       </c>
       <c r="BI18" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BJ18" s="2">
-        <v>-99</v>
-      </c>
-      <c r="BL18" s="5">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="BM18" s="1">
-        <v>2</v>
-      </c>
-      <c r="BN18" s="1">
-        <v>5</v>
-      </c>
-      <c r="BO18" s="1">
-        <v>4</v>
-      </c>
-      <c r="BP18" s="1">
-        <v>5</v>
-      </c>
-      <c r="BQ18" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>0.6875</v>
       </c>
-      <c r="B19" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C19" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D19" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E19" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F19" s="10">
+      <c r="B19" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C19" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D19" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E19" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F19" s="9">
         <v>-50</v>
       </c>
       <c r="H19" s="5">
@@ -6038,16 +4334,16 @@
         <v>0.6875</v>
       </c>
       <c r="AY19" s="1">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="AZ19" s="1">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="BA19" s="1">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="BB19" s="1">
-        <v>-100</v>
+        <v>-99</v>
       </c>
       <c r="BC19" s="2">
         <v>-5</v>
@@ -6056,56 +4352,38 @@
         <v>0.6875</v>
       </c>
       <c r="BF19" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BG19" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BH19" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BI19" s="1">
-        <v>-99</v>
+        <v>4</v>
       </c>
       <c r="BJ19" s="2">
-        <v>-5</v>
-      </c>
-      <c r="BL19" s="5">
-        <v>0.6875</v>
-      </c>
-      <c r="BM19" s="1">
-        <v>3</v>
-      </c>
-      <c r="BN19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BO19" s="1">
-        <v>3</v>
-      </c>
-      <c r="BP19" s="1">
-        <v>4</v>
-      </c>
-      <c r="BQ19" s="2">
         <v>-100</v>
       </c>
     </row>
-    <row r="20" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B20" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C20" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D20" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E20" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F20" s="10">
+      <c r="B20" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C20" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D20" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E20" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F20" s="9">
         <v>-50</v>
       </c>
       <c r="H20" s="5">
@@ -6220,16 +4498,16 @@
         <v>0.70833333333333404</v>
       </c>
       <c r="AY20" s="1">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="AZ20" s="1">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="BA20" s="1">
-        <v>-99</v>
+        <v>4</v>
       </c>
       <c r="BB20" s="1">
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="BC20" s="2">
         <v>-5</v>
@@ -6241,53 +4519,35 @@
         <v>4</v>
       </c>
       <c r="BG20" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BH20" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BI20" s="1">
-        <v>-100</v>
+        <v>3</v>
       </c>
       <c r="BJ20" s="2">
-        <v>-5</v>
-      </c>
-      <c r="BL20" s="5">
-        <v>0.70833333333333404</v>
-      </c>
-      <c r="BM20" s="1">
-        <v>4</v>
-      </c>
-      <c r="BN20" s="1">
-        <v>3</v>
-      </c>
-      <c r="BO20" s="1">
-        <v>2</v>
-      </c>
-      <c r="BP20" s="1">
-        <v>3</v>
-      </c>
-      <c r="BQ20" s="2">
         <v>-100</v>
       </c>
     </row>
-    <row r="21" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>0.72916666666666696</v>
       </c>
-      <c r="B21" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C21" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D21" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E21" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F21" s="10">
+      <c r="B21" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C21" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D21" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E21" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F21" s="9">
         <v>-50</v>
       </c>
       <c r="H21" s="5">
@@ -6402,16 +4662,16 @@
         <v>0.72916666666666696</v>
       </c>
       <c r="AY21" s="1">
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="AZ21" s="1">
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="BA21" s="1">
-        <v>-100</v>
+        <v>3</v>
       </c>
       <c r="BB21" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BC21" s="2">
         <v>-5</v>
@@ -6420,56 +4680,38 @@
         <v>0.72916666666666696</v>
       </c>
       <c r="BF21" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BG21" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH21" s="1">
-        <v>3</v>
+        <v>-100</v>
       </c>
       <c r="BI21" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BJ21" s="2">
-        <v>-5</v>
-      </c>
-      <c r="BL21" s="5">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="BM21" s="1">
-        <v>5</v>
-      </c>
-      <c r="BN21" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO21" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BP21" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ21" s="2">
         <v>-100</v>
       </c>
     </row>
-    <row r="22" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>0.75</v>
       </c>
-      <c r="B22" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C22" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D22" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E22" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F22" s="10">
+      <c r="B22" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C22" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D22" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E22" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F22" s="9">
         <v>-50</v>
       </c>
       <c r="H22" s="5">
@@ -6584,16 +4826,16 @@
         <v>0.75</v>
       </c>
       <c r="AY22" s="1">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="AZ22" s="1">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="BA22" s="1">
-        <v>-100</v>
+        <v>2</v>
       </c>
       <c r="BB22" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BC22" s="2">
         <v>-5</v>
@@ -6602,56 +4844,38 @@
         <v>0.75</v>
       </c>
       <c r="BF22" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BG22" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BH22" s="1">
-        <v>2</v>
+        <v>-100</v>
       </c>
       <c r="BI22" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BJ22" s="2">
-        <v>-5</v>
-      </c>
-      <c r="BL22" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="BM22" s="1">
-        <v>4</v>
-      </c>
-      <c r="BN22" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO22" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BP22" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ22" s="2">
         <v>-100</v>
       </c>
     </row>
-    <row r="23" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>0.77083333333333404</v>
       </c>
-      <c r="B23" s="9">
-        <v>-50</v>
-      </c>
-      <c r="C23" s="9">
-        <v>-50</v>
-      </c>
-      <c r="D23" s="9">
-        <v>-50</v>
-      </c>
-      <c r="E23" s="9">
-        <v>-50</v>
-      </c>
-      <c r="F23" s="10">
+      <c r="B23" s="8">
+        <v>-50</v>
+      </c>
+      <c r="C23" s="8">
+        <v>-50</v>
+      </c>
+      <c r="D23" s="8">
+        <v>-50</v>
+      </c>
+      <c r="E23" s="8">
+        <v>-50</v>
+      </c>
+      <c r="F23" s="9">
         <v>-50</v>
       </c>
       <c r="H23" s="5">
@@ -6766,16 +4990,16 @@
         <v>0.77083333333333404</v>
       </c>
       <c r="AY23" s="1">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="AZ23" s="1">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="BA23" s="1">
-        <v>-100</v>
+        <v>1</v>
       </c>
       <c r="BB23" s="1">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BC23" s="2">
         <v>-5</v>
@@ -6784,56 +5008,38 @@
         <v>0.77083333333333404</v>
       </c>
       <c r="BF23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BG23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH23" s="1">
-        <v>1</v>
+        <v>-100</v>
       </c>
       <c r="BI23" s="1">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BJ23" s="2">
-        <v>-5</v>
-      </c>
-      <c r="BL23" s="5">
-        <v>0.77083333333333404</v>
-      </c>
-      <c r="BM23" s="1">
-        <v>3</v>
-      </c>
-      <c r="BN23" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO23" s="1">
-        <v>-100</v>
-      </c>
-      <c r="BP23" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ23" s="2">
         <v>-100</v>
       </c>
     </row>
-    <row r="24" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B24" s="11">
-        <v>-50</v>
-      </c>
-      <c r="C24" s="11">
-        <v>-50</v>
-      </c>
-      <c r="D24" s="11">
-        <v>-50</v>
-      </c>
-      <c r="E24" s="11">
-        <v>-50</v>
-      </c>
-      <c r="F24" s="12">
+      <c r="B24" s="10">
+        <v>-50</v>
+      </c>
+      <c r="C24" s="10">
+        <v>-50</v>
+      </c>
+      <c r="D24" s="10">
+        <v>-50</v>
+      </c>
+      <c r="E24" s="10">
+        <v>-50</v>
+      </c>
+      <c r="F24" s="11">
         <v>-50</v>
       </c>
       <c r="H24" s="5">
@@ -6948,16 +5154,16 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="AY24" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="AZ24" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BA24" s="3">
-        <v>-99</v>
+        <v>0</v>
       </c>
       <c r="BB24" s="3">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="BC24" s="4">
         <v>-5</v>
@@ -6966,40 +5172,22 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="BF24" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BG24" s="3">
         <v>0</v>
       </c>
       <c r="BH24" s="3">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="BI24" s="3">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="BJ24" s="4">
-        <v>-5</v>
-      </c>
-      <c r="BL24" s="5">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="BM24" s="3">
-        <v>2</v>
-      </c>
-      <c r="BN24" s="3">
-        <v>0</v>
-      </c>
-      <c r="BO24" s="3">
-        <v>-100</v>
-      </c>
-      <c r="BP24" s="3">
-        <v>0</v>
-      </c>
-      <c r="BQ24" s="4">
         <v>-100</v>
       </c>
     </row>
-    <row r="26" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -7011,11 +5199,11 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="1">
         <v>8</v>
       </c>
@@ -7027,11 +5215,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="1">
         <f>C27 + 1</f>
         <v>9</v>
@@ -7042,7 +5230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -7052,7 +5240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -7062,7 +5250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -7074,7 +5262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -7135,243 +5323,243 @@
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
   </mergeCells>
-  <conditionalFormatting sqref="U1:U24 AB1:AB24 AI1:BD24 BR1:XFD24 G1:N24 A27:A28 A25:XFD25 A26:C26 E26:XFD35 A36:XFD1048576 A29:C35 C27:C28">
-    <cfRule type="cellIs" dxfId="159" priority="139" operator="equal">
+  <conditionalFormatting sqref="U1:U24 AB1:AB24 AI1:AW24 BR1:XFD24 G1:N24 A27:A28 A25:XFD25 A26:C26 E26:XFD35 A36:XFD1048576 A29:C35 C27:C28">
+    <cfRule type="cellIs" dxfId="79" priority="139" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="140" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="141" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="142" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="143" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="240" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="241" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:AA1 V8:AA16 V2:V6 V7:Z7 V17:Z24">
-    <cfRule type="cellIs" dxfId="152" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="75" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="76" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="77" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="78" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="79" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="80" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:T24">
-    <cfRule type="cellIs" dxfId="145" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="82" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="83" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="84" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="85" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="86" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="87" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="88" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AH24">
-    <cfRule type="cellIs" dxfId="138" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="67" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="68" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="69" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="70" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="71" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="72" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:AA6">
-    <cfRule type="cellIs" dxfId="131" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="58" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="59" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="60" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="61" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="62" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="63" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="64" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA17:AA24">
-    <cfRule type="cellIs" dxfId="124" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="46" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="47" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="48" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7">
-    <cfRule type="cellIs" dxfId="117" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="39" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U24 AB1:AB24 AI1:BD24 BR1:XFD24 G1:N24 A27:A28 A25:XFD25 A26:C26 E26:XFD35 A36:XFD1048576 A29:C35 C27:C28">
-    <cfRule type="cellIs" dxfId="110" priority="105" operator="equal">
+  <conditionalFormatting sqref="U1:U24 AB1:AB24 AI1:AW24 BR1:XFD24 G1:N24 A27:A28 A25:XFD25 A26:C26 E26:XFD35 A36:XFD1048576 A29:C35 C27:C28">
+    <cfRule type="cellIs" dxfId="30" priority="105" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BK1:BQ24">
-    <cfRule type="cellIs" dxfId="103" priority="26" operator="equal">
+  <conditionalFormatting sqref="BD1:BJ24">
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE1:BJ24">
-    <cfRule type="cellIs" dxfId="96" priority="18" operator="equal">
+  <conditionalFormatting sqref="AX1:BC24">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F24">
-    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F24">
-    <cfRule type="cellIs" dxfId="80" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7484,7 +5672,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="25" operator="containsText" id="{DC4F45F0-A295-4ED3-97E0-2C38404DEA26}">
-            <xm:f>NOT(ISERROR(SEARCH(-5,BK1)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(-5,BD1)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
               <font>
@@ -7497,11 +5685,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>BK1:BQ24</xm:sqref>
+          <xm:sqref>BD1:BJ24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="17" operator="containsText" id="{64681BE5-62F0-4BE2-B713-DF3D34ECA7EB}">
-            <xm:f>NOT(ISERROR(SEARCH(-5,BE1)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(-5,AX1)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
               <font>
@@ -7514,7 +5702,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>BE1:BJ24</xm:sqref>
+          <xm:sqref>AX1:BC24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
final fix and output
</commit_message>
<xml_diff>
--- a/availability.xlsx
+++ b/availability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\GitHub\life-collegia-schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7268CC6C-F0AE-4B64-BA03-8F9C1C51E201}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03809405-07E2-4F1B-9318-F797E3584EF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{750E1001-B131-4AD6-8EA9-0C913AF79012}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{750E1001-B131-4AD6-8EA9-0C913AF79012}"/>
   </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -277,11 +277,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -302,11 +333,635 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="89">
+  <dxfs count="161">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5E913B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4F7EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1544,7 +2199,7 @@
             <v>1</v>
           </cell>
           <cell r="M5">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="P5">
             <v>0</v>
@@ -1592,13 +2247,13 @@
             <v>0</v>
           </cell>
           <cell r="AK5">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="AL5">
             <v>0</v>
           </cell>
           <cell r="AM5">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="AN5">
             <v>0</v>
@@ -1622,7 +2277,7 @@
             <v>0</v>
           </cell>
           <cell r="AY5">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AZ5">
             <v>0</v>
@@ -1634,7 +2289,7 @@
             <v>0</v>
           </cell>
           <cell r="BC5">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="BF5">
             <v>0</v>
@@ -1681,7 +2336,7 @@
             <v>1</v>
           </cell>
           <cell r="M6">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="P6">
             <v>0</v>
@@ -1741,7 +2396,7 @@
             <v>0</v>
           </cell>
           <cell r="AO6">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AR6">
             <v>0</v>
@@ -1759,7 +2414,7 @@
             <v>0</v>
           </cell>
           <cell r="AY6">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AZ6">
             <v>0</v>
@@ -1818,7 +2473,7 @@
             <v>0</v>
           </cell>
           <cell r="M7">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="P7">
             <v>0</v>
@@ -1878,7 +2533,7 @@
             <v>0</v>
           </cell>
           <cell r="AO7">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AR7">
             <v>0</v>
@@ -1896,7 +2551,7 @@
             <v>0</v>
           </cell>
           <cell r="AY7">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AZ7">
             <v>0</v>
@@ -1985,7 +2640,7 @@
             <v>0</v>
           </cell>
           <cell r="AA8">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="AD8">
             <v>0</v>
@@ -2015,7 +2670,7 @@
             <v>0</v>
           </cell>
           <cell r="AO8">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AR8">
             <v>0</v>
@@ -2033,7 +2688,7 @@
             <v>0</v>
           </cell>
           <cell r="AY8">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AZ8">
             <v>0</v>
@@ -2048,7 +2703,7 @@
             <v>0</v>
           </cell>
           <cell r="BF8">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="BG8">
             <v>0</v>
@@ -2122,7 +2777,7 @@
             <v>0</v>
           </cell>
           <cell r="AA9">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="AD9">
             <v>0</v>
@@ -2197,7 +2852,7 @@
             <v>0</v>
           </cell>
           <cell r="BJ9">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="10">
@@ -2259,7 +2914,7 @@
             <v>0</v>
           </cell>
           <cell r="AA10">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="AD10">
             <v>0</v>
@@ -2334,7 +2989,7 @@
             <v>0</v>
           </cell>
           <cell r="BJ10">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="11">
@@ -2920,7 +3575,7 @@
             <v>0</v>
           </cell>
           <cell r="Q15">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="R15">
             <v>1</v>
@@ -2950,7 +3605,7 @@
             <v>1</v>
           </cell>
           <cell r="AE15">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AF15">
             <v>0</v>
@@ -3346,7 +4001,7 @@
             <v>1</v>
           </cell>
           <cell r="X18">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="Y18">
             <v>1</v>
@@ -3406,7 +4061,7 @@
             <v>0</v>
           </cell>
           <cell r="AZ18">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="BA18">
             <v>1</v>
@@ -3477,13 +4132,13 @@
             <v>0</v>
           </cell>
           <cell r="T19">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="W19">
             <v>1</v>
           </cell>
           <cell r="X19">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="Y19">
             <v>1</v>
@@ -3543,7 +4198,7 @@
             <v>0</v>
           </cell>
           <cell r="AZ19">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="BA19">
             <v>1</v>
@@ -3620,7 +4275,7 @@
             <v>1</v>
           </cell>
           <cell r="X20">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="Y20">
             <v>1</v>
@@ -3680,7 +4335,7 @@
             <v>0</v>
           </cell>
           <cell r="AZ20">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="BA20">
             <v>1</v>
@@ -3757,7 +4412,7 @@
             <v>1</v>
           </cell>
           <cell r="X21">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="Y21">
             <v>0</v>
@@ -3817,7 +4472,7 @@
             <v>0</v>
           </cell>
           <cell r="AZ21">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="BA21">
             <v>1</v>
@@ -3891,7 +4546,7 @@
             <v>0</v>
           </cell>
           <cell r="W22">
-            <v>1</v>
+            <v>0</v>
           </cell>
           <cell r="X22">
             <v>0</v>
@@ -4423,7 +5078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2444FAFD-DD66-4923-BB24-9F67C6E049D8}">
   <dimension ref="A1:BJ36"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="67" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="67" workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -8040,167 +8695,167 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="23" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="14">
         <v>-50</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="15">
         <v>-50</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="15">
         <v>-50</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="15">
         <v>-50</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="16">
         <v>-50</v>
       </c>
       <c r="H23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="14">
         <v>-5</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="15">
         <v>-5</v>
       </c>
-      <c r="K23" s="10">
-        <v>-100</v>
-      </c>
-      <c r="L23" s="10">
+      <c r="K23" s="15">
+        <v>-100</v>
+      </c>
+      <c r="L23" s="15">
         <v>-5</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23" s="16">
         <v>-5</v>
       </c>
       <c r="O23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="P23" s="9">
-        <v>-100</v>
-      </c>
-      <c r="Q23" s="10">
-        <v>-100</v>
-      </c>
-      <c r="R23" s="10">
-        <v>-100</v>
-      </c>
-      <c r="S23" s="10">
-        <v>-100</v>
-      </c>
-      <c r="T23" s="3">
+      <c r="P23" s="14">
+        <v>-100</v>
+      </c>
+      <c r="Q23" s="15">
+        <v>-100</v>
+      </c>
+      <c r="R23" s="15">
+        <v>-100</v>
+      </c>
+      <c r="S23" s="15">
+        <v>-100</v>
+      </c>
+      <c r="T23" s="16">
         <v>-100</v>
       </c>
       <c r="V23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="W23" s="9">
+      <c r="W23" s="14">
         <v>2</v>
       </c>
-      <c r="X23" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="3">
+      <c r="X23" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="16">
         <v>-5</v>
       </c>
       <c r="AC23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="AD23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AF23" s="10">
+      <c r="AD23" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="15">
         <v>-5</v>
       </c>
-      <c r="AG23" s="10">
+      <c r="AG23" s="15">
         <v>-5</v>
       </c>
-      <c r="AH23" s="3">
+      <c r="AH23" s="16">
         <v>4</v>
       </c>
       <c r="AJ23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="AK23" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL23" s="10">
+      <c r="AK23" s="14">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="15">
         <v>4</v>
       </c>
-      <c r="AM23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AN23" s="10">
-        <v>-100</v>
-      </c>
-      <c r="AO23" s="3">
+      <c r="AM23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN23" s="15">
+        <v>-100</v>
+      </c>
+      <c r="AO23" s="16">
         <v>1</v>
       </c>
       <c r="AQ23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="AR23" s="9">
-        <v>-100</v>
-      </c>
-      <c r="AS23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AT23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AU23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AV23" s="3">
+      <c r="AR23" s="14">
+        <v>-100</v>
+      </c>
+      <c r="AS23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AT23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AU23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AV23" s="16">
         <v>-5</v>
       </c>
       <c r="AX23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="AY23" s="9">
-        <v>1</v>
-      </c>
-      <c r="AZ23" s="10">
-        <v>1</v>
-      </c>
-      <c r="BA23" s="10">
-        <v>1</v>
-      </c>
-      <c r="BB23" s="10">
-        <v>-100</v>
-      </c>
-      <c r="BC23" s="3">
+      <c r="AY23" s="14">
+        <v>1</v>
+      </c>
+      <c r="AZ23" s="15">
+        <v>1</v>
+      </c>
+      <c r="BA23" s="15">
+        <v>1</v>
+      </c>
+      <c r="BB23" s="15">
+        <v>-100</v>
+      </c>
+      <c r="BC23" s="16">
         <v>-5</v>
       </c>
       <c r="BE23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="BF23" s="9">
+      <c r="BF23" s="14">
         <v>3</v>
       </c>
-      <c r="BG23" s="10">
-        <v>0</v>
-      </c>
-      <c r="BH23" s="10">
-        <v>-100</v>
-      </c>
-      <c r="BI23" s="10">
-        <v>0</v>
-      </c>
-      <c r="BJ23" s="3">
+      <c r="BG23" s="15">
+        <v>0</v>
+      </c>
+      <c r="BH23" s="15">
+        <v>-100</v>
+      </c>
+      <c r="BI23" s="15">
+        <v>0</v>
+      </c>
+      <c r="BJ23" s="16">
         <v>-100</v>
       </c>
     </row>
@@ -8335,15 +8990,18 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
       <c r="H36" s="1">
         <v>-50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="E36:G36"/>
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="E35:G35"/>
@@ -8354,306 +9012,530 @@
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
   </mergeCells>
-  <conditionalFormatting sqref="U1:U23 AB1:AB23 AI1:AI23 BR1:XFD23 G1:G23 A27:A28 A24:XFD25 A26:C26 A29:C35 C27:C28 N1:N23 AP1:AP23 AW1:AW23 E28:F30 H27:XFD36 A37:XFD1048576 A36:F36 E26:E27 E31:E35 I26:XFD26">
-    <cfRule type="cellIs" dxfId="88" priority="211" operator="equal">
+  <conditionalFormatting sqref="U1:U23 AB1:AB23 AI1:AI23 BR1:XFD23 G1:G23 A27:A28 A24:XFD25 A26:C26 A29:C35 C27:C28 N1:N23 AP1:AP23 AW1:AW23 E28:F30 H27:XFD36 A37:XFD1048576 A36:E36 E26:E27 E31:E35 I26:XFD26">
+    <cfRule type="cellIs" dxfId="160" priority="283" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="284" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="285" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="286" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="287" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="312" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="384" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="313" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="385" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U23 AB1:AB23 AI1:AI23 BR1:XFD23 G1:G23 A27:A28 A24:XFD25 A26:C26 A29:C35 C27:C28 N1:N23 AP1:AP23 AW1:AW23 E28:F30 H27:XFD36 A37:XFD1048576 A36:F36 E26:E27 E31:E35 I26:XFD26">
-    <cfRule type="cellIs" dxfId="81" priority="177" operator="equal">
+  <conditionalFormatting sqref="U1:U23 AB1:AB23 AI1:AI23 BR1:XFD23 G1:G23 A27:A28 A24:XFD25 A26:C26 A29:C35 C27:C28 N1:N23 AP1:AP23 AW1:AW23 E28:F30 H27:XFD36 A37:XFD1048576 A36:E36 E26:E27 E31:E35 I26:XFD26">
+    <cfRule type="cellIs" dxfId="153" priority="249" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD1:BD23">
-    <cfRule type="cellIs" dxfId="80" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="170" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="171" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="172" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="173" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="174" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="175" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="176" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F23">
-    <cfRule type="cellIs" dxfId="73" priority="74" operator="equal">
+  <conditionalFormatting sqref="A1:F1 A2:A23">
+    <cfRule type="cellIs" dxfId="145" priority="146" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="147" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="148" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="149" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="150" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="151" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="152" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F23">
-    <cfRule type="cellIs" dxfId="66" priority="73" operator="equal">
+  <conditionalFormatting sqref="A1:F1 A2:A23">
+    <cfRule type="cellIs" dxfId="138" priority="145" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:M23">
-    <cfRule type="cellIs" dxfId="65" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="130" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="131" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="132" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="133" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="134" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="135" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="136" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:M23">
-    <cfRule type="cellIs" dxfId="58" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="129" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T23">
-    <cfRule type="cellIs" dxfId="57" priority="50" operator="equal">
+  <conditionalFormatting sqref="O1:T1 O2:O23">
+    <cfRule type="cellIs" dxfId="129" priority="122" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="123" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="124" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="125" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="126" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="127" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="128" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T23">
-    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+  <conditionalFormatting sqref="O1:T1 O2:O23">
+    <cfRule type="cellIs" dxfId="122" priority="121" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:AA23">
-    <cfRule type="cellIs" dxfId="49" priority="42" operator="equal">
+  <conditionalFormatting sqref="V1:AA1 V2:V23">
+    <cfRule type="cellIs" dxfId="121" priority="114" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="115" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="116" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="117" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="118" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="119" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="120" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:AA23">
-    <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
+  <conditionalFormatting sqref="V1:AA1 V2:V23">
+    <cfRule type="cellIs" dxfId="114" priority="113" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC1:AH23">
-    <cfRule type="cellIs" dxfId="41" priority="34" operator="equal">
+  <conditionalFormatting sqref="AC1:AH1 AC2:AC23">
+    <cfRule type="cellIs" dxfId="113" priority="106" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="107" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="108" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="109" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="110" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="111" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="112" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC1:AH23">
-    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
+  <conditionalFormatting sqref="AC1:AH1 AC2:AC23">
+    <cfRule type="cellIs" dxfId="106" priority="105" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ1:AO23">
-    <cfRule type="cellIs" dxfId="33" priority="26" operator="equal">
+  <conditionalFormatting sqref="AJ1:AO1 AJ2:AJ23">
+    <cfRule type="cellIs" dxfId="105" priority="98" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="99" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="100" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="101" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="102" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="103" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="104" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ1:AO23">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+  <conditionalFormatting sqref="AJ1:AO1 AJ2:AJ23">
+    <cfRule type="cellIs" dxfId="98" priority="97" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ1:AV23">
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
+  <conditionalFormatting sqref="AQ1:AV1 AQ2:AQ23">
+    <cfRule type="cellIs" dxfId="97" priority="90" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="91" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="92" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="93" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="94" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="95" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="96" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ1:AV23">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+  <conditionalFormatting sqref="AQ1:AV1 AQ2:AQ23">
+    <cfRule type="cellIs" dxfId="90" priority="89" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AX1:BC23">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+  <conditionalFormatting sqref="AX1:BC1 AX2:AX23">
+    <cfRule type="cellIs" dxfId="89" priority="82" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="83" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="84" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="85" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="86" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="87" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AX1:BC23">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+  <conditionalFormatting sqref="AX1:BC1 AX2:AX23">
+    <cfRule type="cellIs" dxfId="82" priority="81" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE1:BJ23">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+  <conditionalFormatting sqref="BE1:BJ1 BE2:BE23">
+    <cfRule type="cellIs" dxfId="81" priority="74" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="75" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="76" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="77" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="78" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="79" operator="equal">
       <formula>-99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="80" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE1:BJ23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="BE1:BJ1 BE2:BE23">
+    <cfRule type="cellIs" dxfId="74" priority="73" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:F23">
+    <cfRule type="cellIs" dxfId="71" priority="66" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="67" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="68" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="69" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="70" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="71" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="72" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:F23">
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:T23">
+    <cfRule type="cellIs" dxfId="55" priority="50" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="51" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="56" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:T23">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:AA23">
+    <cfRule type="cellIs" dxfId="47" priority="42" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="47" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="48" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:AA23">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD2:AH23">
+    <cfRule type="cellIs" dxfId="39" priority="34" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="36" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="40" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD2:AH23">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK2:AO23">
+    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK2:AO23">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR2:AV23">
+    <cfRule type="cellIs" dxfId="23" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="24" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR2:AV23">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY2:BC23">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY2:BC23">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>-5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BF2:BJ23">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+      <formula>-99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BF2:BJ23">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8663,7 +9545,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="97" operator="containsText" id="{DC4F45F0-A295-4ED3-97E0-2C38404DEA26}">
+          <x14:cfRule type="containsText" priority="169" operator="containsText" id="{DC4F45F0-A295-4ED3-97E0-2C38404DEA26}">
             <xm:f>NOT(ISERROR(SEARCH(-5,BD1)))</xm:f>
             <xm:f>-5</xm:f>
             <x14:dxf>
@@ -8689,8 +9571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4F6A99-AA84-4FE6-9BCF-1526F392FAD1}">
   <dimension ref="A1:BJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="I1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="BF2" sqref="BF2:BJ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9534,7 +10416,7 @@
       </c>
       <c r="M5" s="3">
         <f>[1]Assignments!M5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="4">
         <v>0.39583333333333298</v>
@@ -9610,7 +10492,7 @@
       </c>
       <c r="AK5" s="9">
         <f>[1]Assignments!AK5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL5" s="10">
         <f>[1]Assignments!AL5</f>
@@ -9618,7 +10500,7 @@
       </c>
       <c r="AM5" s="10">
         <f>[1]Assignments!AM5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN5" s="10">
         <f>[1]Assignments!AN5</f>
@@ -9656,7 +10538,7 @@
       </c>
       <c r="AY5" s="9">
         <f>[1]Assignments!AY5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ5" s="10">
         <f>[1]Assignments!AZ5</f>
@@ -9672,7 +10554,7 @@
       </c>
       <c r="BC5" s="3">
         <f>[1]Assignments!BC5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE5" s="4">
         <v>0.39583333333333298</v>
@@ -9743,7 +10625,7 @@
       </c>
       <c r="M6" s="3">
         <f>[1]Assignments!M6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" s="4">
         <v>0.41666666666666702</v>
@@ -9835,7 +10717,7 @@
       </c>
       <c r="AO6" s="3">
         <f>[1]Assignments!AO6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="4">
         <v>0.41666666666666702</v>
@@ -9865,7 +10747,7 @@
       </c>
       <c r="AY6" s="9">
         <f>[1]Assignments!AY6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ6" s="10">
         <f>[1]Assignments!AZ6</f>
@@ -9952,7 +10834,7 @@
       </c>
       <c r="M7" s="3">
         <f>[1]Assignments!M7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="4">
         <v>0.4375</v>
@@ -10044,7 +10926,7 @@
       </c>
       <c r="AO7" s="3">
         <f>[1]Assignments!AO7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ7" s="4">
         <v>0.4375</v>
@@ -10074,7 +10956,7 @@
       </c>
       <c r="AY7" s="9">
         <f>[1]Assignments!AY7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ7" s="10">
         <f>[1]Assignments!AZ7</f>
@@ -10207,7 +11089,7 @@
       </c>
       <c r="AA8" s="3">
         <f>[1]Assignments!AA8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="4">
         <v>0.45833333333333298</v>
@@ -10253,7 +11135,7 @@
       </c>
       <c r="AO8" s="3">
         <f>[1]Assignments!AO8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ8" s="4">
         <v>0.45833333333333298</v>
@@ -10283,7 +11165,7 @@
       </c>
       <c r="AY8" s="9">
         <f>[1]Assignments!AY8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ8" s="10">
         <f>[1]Assignments!AZ8</f>
@@ -10306,7 +11188,7 @@
       </c>
       <c r="BF8" s="9">
         <f>[1]Assignments!BF8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG8" s="10">
         <f>[1]Assignments!BG8</f>
@@ -10416,7 +11298,7 @@
       </c>
       <c r="AA9" s="3">
         <f>[1]Assignments!AA9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="4">
         <v>0.47916666666666702</v>
@@ -10531,7 +11413,7 @@
       </c>
       <c r="BJ9" s="3">
         <f>[1]Assignments!BJ9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.3">
@@ -10625,7 +11507,7 @@
       </c>
       <c r="AA10" s="3">
         <f>[1]Assignments!AA10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="4">
         <v>0.5</v>
@@ -10740,7 +11622,7 @@
       </c>
       <c r="BJ10" s="3">
         <f>[1]Assignments!BJ10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
@@ -11635,7 +12517,7 @@
       </c>
       <c r="Q15" s="10">
         <f>[1]Assignments!Q15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="10">
         <f>[1]Assignments!R15</f>
@@ -11681,7 +12563,7 @@
       </c>
       <c r="AE15" s="10">
         <f>[1]Assignments!AE15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15" s="10">
         <f>[1]Assignments!AF15</f>
@@ -12285,7 +13167,7 @@
       </c>
       <c r="X18" s="10">
         <f>[1]Assignments!X18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y18" s="10">
         <f>[1]Assignments!Y18</f>
@@ -12377,7 +13259,7 @@
       </c>
       <c r="AZ18" s="10">
         <f>[1]Assignments!AZ18</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA18" s="10">
         <f>[1]Assignments!BA18</f>
@@ -12483,7 +13365,7 @@
       </c>
       <c r="T19" s="3">
         <f>[1]Assignments!T19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" s="4">
         <v>0.6875</v>
@@ -12494,7 +13376,7 @@
       </c>
       <c r="X19" s="10">
         <f>[1]Assignments!X19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" s="10">
         <f>[1]Assignments!Y19</f>
@@ -12586,7 +13468,7 @@
       </c>
       <c r="AZ19" s="10">
         <f>[1]Assignments!AZ19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA19" s="10">
         <f>[1]Assignments!BA19</f>
@@ -12703,7 +13585,7 @@
       </c>
       <c r="X20" s="10">
         <f>[1]Assignments!X20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y20" s="10">
         <f>[1]Assignments!Y20</f>
@@ -12795,7 +13677,7 @@
       </c>
       <c r="AZ20" s="10">
         <f>[1]Assignments!AZ20</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA20" s="10">
         <f>[1]Assignments!BA20</f>
@@ -12912,7 +13794,7 @@
       </c>
       <c r="X21" s="10">
         <f>[1]Assignments!X21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21" s="10">
         <f>[1]Assignments!Y21</f>
@@ -13004,7 +13886,7 @@
       </c>
       <c r="AZ21" s="10">
         <f>[1]Assignments!AZ21</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA21" s="10">
         <f>[1]Assignments!BA21</f>
@@ -13117,7 +13999,7 @@
       </c>
       <c r="W22" s="9">
         <f>[1]Assignments!W22</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22" s="10">
         <f>[1]Assignments!X22</f>
@@ -13251,211 +14133,211 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="14">
         <f>[1]Assignments!B23</f>
         <v>0</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="15">
         <f>[1]Assignments!C23</f>
         <v>0</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="15">
         <f>[1]Assignments!D23</f>
         <v>0</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="15">
         <f>[1]Assignments!E23</f>
         <v>0</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="16">
         <f>[1]Assignments!F23</f>
         <v>0</v>
       </c>
       <c r="H23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="14">
         <f>[1]Assignments!I23</f>
         <v>0</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="15">
         <f>[1]Assignments!J23</f>
         <v>0</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="15">
         <f>[1]Assignments!K23</f>
         <v>0</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="15">
         <f>[1]Assignments!L23</f>
         <v>1</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23" s="16">
         <f>[1]Assignments!M23</f>
         <v>0</v>
       </c>
       <c r="O23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="P23" s="9">
+      <c r="P23" s="14">
         <f>[1]Assignments!P23</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="10">
+      <c r="Q23" s="15">
         <f>[1]Assignments!Q23</f>
         <v>0</v>
       </c>
-      <c r="R23" s="10">
+      <c r="R23" s="15">
         <f>[1]Assignments!R23</f>
         <v>0</v>
       </c>
-      <c r="S23" s="10">
+      <c r="S23" s="15">
         <f>[1]Assignments!S23</f>
         <v>0</v>
       </c>
-      <c r="T23" s="3">
+      <c r="T23" s="16">
         <f>[1]Assignments!T23</f>
         <v>0</v>
       </c>
       <c r="V23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="W23" s="9">
+      <c r="W23" s="14">
         <f>[1]Assignments!W23</f>
         <v>0</v>
       </c>
-      <c r="X23" s="10">
+      <c r="X23" s="15">
         <f>[1]Assignments!X23</f>
         <v>0</v>
       </c>
-      <c r="Y23" s="10">
+      <c r="Y23" s="15">
         <f>[1]Assignments!Y23</f>
         <v>0</v>
       </c>
-      <c r="Z23" s="10">
+      <c r="Z23" s="15">
         <f>[1]Assignments!Z23</f>
         <v>0</v>
       </c>
-      <c r="AA23" s="3">
+      <c r="AA23" s="16">
         <f>[1]Assignments!AA23</f>
         <v>0</v>
       </c>
       <c r="AC23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="AD23" s="9">
+      <c r="AD23" s="14">
         <f>[1]Assignments!AD23</f>
         <v>0</v>
       </c>
-      <c r="AE23" s="10">
+      <c r="AE23" s="15">
         <f>[1]Assignments!AE23</f>
         <v>0</v>
       </c>
-      <c r="AF23" s="10">
+      <c r="AF23" s="15">
         <f>[1]Assignments!AF23</f>
         <v>0</v>
       </c>
-      <c r="AG23" s="10">
+      <c r="AG23" s="15">
         <f>[1]Assignments!AG23</f>
         <v>0</v>
       </c>
-      <c r="AH23" s="3">
+      <c r="AH23" s="16">
         <f>[1]Assignments!AH23</f>
         <v>1</v>
       </c>
       <c r="AJ23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="AK23" s="9">
+      <c r="AK23" s="14">
         <f>[1]Assignments!AK23</f>
         <v>0</v>
       </c>
-      <c r="AL23" s="10">
+      <c r="AL23" s="15">
         <f>[1]Assignments!AL23</f>
         <v>1</v>
       </c>
-      <c r="AM23" s="10">
+      <c r="AM23" s="15">
         <f>[1]Assignments!AM23</f>
         <v>0</v>
       </c>
-      <c r="AN23" s="10">
+      <c r="AN23" s="15">
         <f>[1]Assignments!AN23</f>
         <v>0</v>
       </c>
-      <c r="AO23" s="3">
+      <c r="AO23" s="16">
         <f>[1]Assignments!AO23</f>
         <v>0</v>
       </c>
       <c r="AQ23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="AR23" s="9">
+      <c r="AR23" s="14">
         <f>[1]Assignments!AR23</f>
         <v>0</v>
       </c>
-      <c r="AS23" s="10">
+      <c r="AS23" s="15">
         <f>[1]Assignments!AS23</f>
         <v>0</v>
       </c>
-      <c r="AT23" s="10">
+      <c r="AT23" s="15">
         <f>[1]Assignments!AT23</f>
         <v>0</v>
       </c>
-      <c r="AU23" s="10">
+      <c r="AU23" s="15">
         <f>[1]Assignments!AU23</f>
         <v>0</v>
       </c>
-      <c r="AV23" s="3">
+      <c r="AV23" s="16">
         <f>[1]Assignments!AV23</f>
         <v>0</v>
       </c>
       <c r="AX23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="AY23" s="9">
+      <c r="AY23" s="14">
         <f>[1]Assignments!AY23</f>
         <v>0</v>
       </c>
-      <c r="AZ23" s="10">
+      <c r="AZ23" s="15">
         <f>[1]Assignments!AZ23</f>
         <v>0</v>
       </c>
-      <c r="BA23" s="10">
+      <c r="BA23" s="15">
         <f>[1]Assignments!BA23</f>
         <v>1</v>
       </c>
-      <c r="BB23" s="10">
+      <c r="BB23" s="15">
         <f>[1]Assignments!BB23</f>
         <v>0</v>
       </c>
-      <c r="BC23" s="3">
+      <c r="BC23" s="16">
         <f>[1]Assignments!BC23</f>
         <v>0</v>
       </c>
       <c r="BE23" s="4">
         <v>0.77083333333333404</v>
       </c>
-      <c r="BF23" s="9">
+      <c r="BF23" s="14">
         <f>[1]Assignments!BF23</f>
         <v>1</v>
       </c>
-      <c r="BG23" s="10">
+      <c r="BG23" s="15">
         <f>[1]Assignments!BG23</f>
         <v>0</v>
       </c>
-      <c r="BH23" s="10">
+      <c r="BH23" s="15">
         <f>[1]Assignments!BH23</f>
         <v>0</v>
       </c>
-      <c r="BI23" s="10">
+      <c r="BI23" s="15">
         <f>[1]Assignments!BI23</f>
         <v>0</v>
       </c>
-      <c r="BJ23" s="3">
+      <c r="BJ23" s="16">
         <f>[1]Assignments!BJ23</f>
         <v>0</v>
       </c>
@@ -13561,7 +14443,7 @@
     <mergeCell ref="A26:C26"/>
   </mergeCells>
   <conditionalFormatting sqref="A27:XFD1048576 A26 D26:XFD26 A1:XFD25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>